<commit_message>
booknow mobile not fixed
</commit_message>
<xml_diff>
--- a/assets/dataFiles/sliderref.xlsx
+++ b/assets/dataFiles/sliderref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anjankumar.bnv\Documents\myproject\ootytaxi\assets\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F4B75-E848-49C2-8FB6-3CFCE930568D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41AE469-465A-4AE1-9226-2D98D7CA8D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{A56E54FD-08BE-470A-B68D-7B09EA6BE3DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{A56E54FD-08BE-470A-B68D-7B09EA6BE3DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Ooty" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t>Path</t>
   </si>
@@ -64,40 +64,166 @@
     <t>5.jpg</t>
   </si>
   <si>
-    <t>Ooty Park</t>
-  </si>
-  <si>
-    <t>A Beautiful View</t>
-  </si>
-  <si>
-    <t>Theme Park</t>
-  </si>
-  <si>
-    <t>What Else</t>
-  </si>
-  <si>
-    <t>Botanical Garden</t>
-  </si>
-  <si>
     <t>Image Filename</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua.</t>
-  </si>
-  <si>
     <t>assets/images/myslider/ooty/</t>
   </si>
   <si>
-    <t>Coonoor</t>
-  </si>
-  <si>
-    <t>Mysore</t>
-  </si>
-  <si>
-    <t>Munnar</t>
-  </si>
-  <si>
-    <t>Kotagiri</t>
+    <t>Escape to Ooty: A Natural Paradise in the Hills</t>
+  </si>
+  <si>
+    <t>Nestled in the Western Ghats, Ooty offers visitors a serene escape to lush landscapes, winding trails, and cascading waterfalls. Discover the best of this charming hill station in our comprehensive travel guide.</t>
+  </si>
+  <si>
+    <t>Beyond the tourist traps, Ooty has a treasure trove of lesser-known attractions waiting to be explored. From serene botanical gardens to colonial-era bungalows, discover the hidden gems of this hill station.</t>
+  </si>
+  <si>
+    <t>Ooty's Hidden Gems: Uncovering the Charms of the Queen of Hill Stations</t>
+  </si>
+  <si>
+    <t>A Journey Back in Time: Exploring Ooty's Colonial Legacy</t>
+  </si>
+  <si>
+    <t>Step back in time to the days of the Raj as you explore Ooty's colonial-era architecture, historic churches, and charming tea plantations. Our guide takes you on a journey through the town's rich history.</t>
+  </si>
+  <si>
+    <t>Ooty for the Adventurous: Exploring the Great Outdoors</t>
+  </si>
+  <si>
+    <t>For outdoor enthusiasts, Ooty offers endless opportunities for trekking, mountain biking, and wildlife spotting. Get ready to take on the great outdoors in this thrilling hill station.</t>
+  </si>
+  <si>
+    <t>The Ultimate Guide to Ooty: Planning Your Perfect Getaway</t>
+  </si>
+  <si>
+    <t>Planning a trip to Ooty? Our comprehensive guide has everything you need to know, from the best time to visit and top attractions to where to stay and what to eat. Start planning your dream getaway today!</t>
+  </si>
+  <si>
+    <t>Discover the Hidden Gem of the Nilgiris: Coonoor Visitor Guide</t>
+  </si>
+  <si>
+    <t>Explore the charming hill town of Coonoor and its tea estates, scenic vistas, and historic landmarks. This guide offers insider tips on the best places to visit, stay, and dine in Coonoor.</t>
+  </si>
+  <si>
+    <t>Escape to the Serene Beauty of Coonoor: A Visitor's Delight</t>
+  </si>
+  <si>
+    <t>Indulge in the tranquility of Coonoor's lush landscapes and pleasant weather. This visitor's guide will take you on a tour of the picturesque hills, tea gardens, and nature reserves of Coonoor.</t>
+  </si>
+  <si>
+    <t>Coonoor: A Journey to the Land of the Eternal Spring</t>
+  </si>
+  <si>
+    <t>Immerse yourself in the temperate climate, rolling hills, and verdant forests of Coonoor. This guide will lead you on a journey through Coonoor's lush environs, picturesque gardens, and charming town center.</t>
+  </si>
+  <si>
+    <t>Step into the Past: A Historical Tour of Coonoor Visitors' Highlights</t>
+  </si>
+  <si>
+    <t>Uncover Coonoor's rich heritage with a visit to its colonial architecture, vintage toy train, and historic landmarks. This guide will take you on a journey through Coonoor's colorful past and its enduring landmarks.</t>
+  </si>
+  <si>
+    <t>Coonoor: A Culinary Journey to the Hills</t>
+  </si>
+  <si>
+    <t>Experience Coonoor's distinctive cuisine, featuring an array of tea-infused dishes and authentic South Indian delicacies. This guide will introduce you to the best restaurants, cafes, and tea rooms in Coonoor.</t>
+  </si>
+  <si>
+    <t>Discovering the Hidden Gems of Kotagiri: A Travel Guide</t>
+  </si>
+  <si>
+    <t>Explore the scenic town of Kotagiri, nestled in the Nilgiri Hills of Tamil Nadu, India. From hiking to tea plantations and waterfalls to exploring local culture and cuisine, this travel guide will help you make the most of your visit to Kotagiri.</t>
+  </si>
+  <si>
+    <t>Kotagiri: A Serene Hill Station Retreat</t>
+  </si>
+  <si>
+    <t>Escape the hustle and bustle of city life and retreat to the tranquil hills of Kotagiri. Enjoy breathtaking views of the lush landscape, explore quaint villages, and rejuvenate your mind and body in the serene environment.</t>
+  </si>
+  <si>
+    <t>Uncovering the History and Heritage of Kotagiri</t>
+  </si>
+  <si>
+    <t>Step back in time and discover the rich history and heritage of Kotagiri. Explore ancient temples, colonial architecture, and museums that showcase the town's fascinating past.</t>
+  </si>
+  <si>
+    <t>Kotagiri: A Foodie's Paradise</t>
+  </si>
+  <si>
+    <t>Savor the flavors of Kotagiri's vibrant cuisine, which blends traditional South Indian dishes with colonial and European influences. From local street food to fine dining restaurants, there's something for every foodie in Kotagiri.</t>
+  </si>
+  <si>
+    <t>Adventure Awaits: Exploring the Great Outdoors of Kotagiri</t>
+  </si>
+  <si>
+    <t>Get your adrenaline pumping with thrilling outdoor activities in Kotagiri. Go trekking, rock climbing, mountain biking, or paragliding and experience the natural beauty of the town from a new perspective.</t>
+  </si>
+  <si>
+    <t>Munnar: The Blissful Hill Station in God's Own Country</t>
+  </si>
+  <si>
+    <t>Discover the picturesque hills of Munnar and immerse yourself in the tranquil beauty of this popular tourist destination in Kerala.</t>
+  </si>
+  <si>
+    <t>Exploring Munnar's Tea Plantations: A Journey Through the Fragrant Landscapes</t>
+  </si>
+  <si>
+    <t>Get lost in the scenic tea plantations of Munnar and experience the aroma of fresh tea leaves in the air.</t>
+  </si>
+  <si>
+    <t>Munnar's Top Attractions: A Must-Visit Guide</t>
+  </si>
+  <si>
+    <t>Discover the must-see attractions in Munnar, from cascading waterfalls to wildlife sanctuaries and stunning viewpoints.</t>
+  </si>
+  <si>
+    <t>Unwind in Munnar's Serene Nature: A Perfect Getaway from the City Life</t>
+  </si>
+  <si>
+    <t>Escape the hustle and bustle of city life and find your inner peace in the natural beauty of Munnar.</t>
+  </si>
+  <si>
+    <t>Adventure and Thrills in Munnar: A Paradise for Outdoor Enthusiasts</t>
+  </si>
+  <si>
+    <t>Embark on an exciting journey filled with adventure and adrenaline in Munnar, where you can trek, camp, and explore to your heart's content.</t>
+  </si>
+  <si>
+    <t>Majestic Mysore: Exploring the Palace City of Karnataka</t>
+  </si>
+  <si>
+    <t>Discover the grandeur of Mysore, home to the magnificent Mysore Palace and other architectural wonders.</t>
+  </si>
+  <si>
+    <t>Immerse yourself in Mysore's rich culture through its vibrant festivals, traditional crafts, and delectable cuisine.</t>
+  </si>
+  <si>
+    <t>Venture off the beaten path and discover the lesser-known attractions of Mysore, such as the tranquil Brindavan Gardens and the historic Jaganmohan Palace.</t>
+  </si>
+  <si>
+    <t>Take a journey through Mysore's royal past and learn about the legacy of the Wodeyar dynasty, which ruled the region for centuries.</t>
+  </si>
+  <si>
+    <t>Escape the city bustle and discover the natural beauty of Mysore's surrounding hills, forests, and wildlife reserves, such as the Nagarhole National Park and the Chamundi Hills.</t>
+  </si>
+  <si>
+    <t>Nature's Bounty in Mysore: Exploring the City's Surrounding Hills and Wildlife Reserves</t>
+  </si>
+  <si>
+    <t>Mysore's Royal Legacy: Tracing the Footsteps of the Wodeyars</t>
+  </si>
+  <si>
+    <t>Beyond the Palace Gates: Uncovering Hidden Gems in Mysore</t>
+  </si>
+  <si>
+    <t>The Cultural Capital of Karnataka: A Guide to Mysore's Festivals and Traditions</t>
+  </si>
+  <si>
+    <t>assets/images/myslider/coonoor/</t>
+  </si>
+  <si>
+    <t>assets/images/myslider/mysore/</t>
   </si>
 </sst>
 </file>
@@ -455,7 +581,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,80 +600,80 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -560,11 +686,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD43960-86A8-4F84-BE55-4FB2AE2562EF}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="4" max="4" width="114.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -574,84 +704,85 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -660,10 +791,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -673,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -681,72 +815,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -758,11 +892,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29CC478-6A98-47F3-84DB-DB2CB8A0A8E4}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -772,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -780,72 +915,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +993,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -871,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -879,72 +1017,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>